<commit_message>
More updates to character tables, analysis.
</commit_message>
<xml_diff>
--- a/notes/char-table.xlsx
+++ b/notes/char-table.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12640" yWindow="0" windowWidth="14880" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="17140" yWindow="0" windowWidth="11660" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
+    <sheet name="RTM Both" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="1451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2465" uniqueCount="1451">
   <si>
     <t>Character</t>
   </si>
@@ -4420,8 +4421,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4474,7 +4481,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4497,6 +4504,9 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4519,6 +4529,9 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4850,9 +4863,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K289"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E243" sqref="E243"/>
+      <selection pane="bottomLeft" activeCell="B273" sqref="B273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9436,6 +9449,9 @@
       <c r="A205" s="1" t="s">
         <v>1284</v>
       </c>
+      <c r="B205" t="s">
+        <v>78</v>
+      </c>
       <c r="E205" t="s">
         <v>1418</v>
       </c>
@@ -9453,6 +9469,9 @@
       <c r="A206" s="1" t="s">
         <v>1301</v>
       </c>
+      <c r="B206" t="s">
+        <v>44</v>
+      </c>
       <c r="E206" t="s">
         <v>1419</v>
       </c>
@@ -9470,6 +9489,9 @@
       <c r="A207" s="1" t="s">
         <v>1291</v>
       </c>
+      <c r="B207" t="s">
+        <v>78</v>
+      </c>
       <c r="E207" t="s">
         <v>1420</v>
       </c>
@@ -9487,6 +9509,9 @@
       <c r="A208" s="1" t="s">
         <v>1308</v>
       </c>
+      <c r="B208" t="s">
+        <v>44</v>
+      </c>
       <c r="E208" t="s">
         <v>1421</v>
       </c>
@@ -9504,6 +9529,9 @@
       <c r="A209" s="1" t="s">
         <v>1292</v>
       </c>
+      <c r="B209" t="s">
+        <v>78</v>
+      </c>
       <c r="E209" t="s">
         <v>1422</v>
       </c>
@@ -9521,6 +9549,9 @@
       <c r="A210" s="1" t="s">
         <v>1309</v>
       </c>
+      <c r="B210" t="s">
+        <v>44</v>
+      </c>
       <c r="E210" t="s">
         <v>1423</v>
       </c>
@@ -9538,6 +9569,9 @@
       <c r="A211" s="1" t="s">
         <v>1277</v>
       </c>
+      <c r="B211" t="s">
+        <v>78</v>
+      </c>
       <c r="E211" t="s">
         <v>1424</v>
       </c>
@@ -9555,6 +9589,9 @@
       <c r="A212" s="1" t="s">
         <v>1294</v>
       </c>
+      <c r="B212" t="s">
+        <v>44</v>
+      </c>
       <c r="E212" t="s">
         <v>1425</v>
       </c>
@@ -9572,6 +9609,9 @@
       <c r="A213" s="1" t="s">
         <v>1278</v>
       </c>
+      <c r="B213" t="s">
+        <v>78</v>
+      </c>
       <c r="E213" t="s">
         <v>1426</v>
       </c>
@@ -9589,6 +9629,9 @@
       <c r="A214" s="1" t="s">
         <v>1295</v>
       </c>
+      <c r="B214" t="s">
+        <v>44</v>
+      </c>
       <c r="E214" t="s">
         <v>1427</v>
       </c>
@@ -9606,6 +9649,9 @@
       <c r="A215" s="1" t="s">
         <v>1279</v>
       </c>
+      <c r="B215" t="s">
+        <v>78</v>
+      </c>
       <c r="E215" t="s">
         <v>1428</v>
       </c>
@@ -9623,6 +9669,9 @@
       <c r="A216" s="1" t="s">
         <v>1296</v>
       </c>
+      <c r="B216" t="s">
+        <v>44</v>
+      </c>
       <c r="E216" t="s">
         <v>1429</v>
       </c>
@@ -9640,6 +9689,9 @@
       <c r="A217" s="1" t="s">
         <v>1282</v>
       </c>
+      <c r="B217" t="s">
+        <v>78</v>
+      </c>
       <c r="E217" t="s">
         <v>1430</v>
       </c>
@@ -9657,6 +9709,9 @@
       <c r="A218" s="1" t="s">
         <v>1299</v>
       </c>
+      <c r="B218" t="s">
+        <v>44</v>
+      </c>
       <c r="E218" t="s">
         <v>1431</v>
       </c>
@@ -9674,6 +9729,9 @@
       <c r="A219" s="1" t="s">
         <v>1281</v>
       </c>
+      <c r="B219" t="s">
+        <v>78</v>
+      </c>
       <c r="E219" t="s">
         <v>1432</v>
       </c>
@@ -9691,6 +9749,9 @@
       <c r="A220" s="1" t="s">
         <v>1298</v>
       </c>
+      <c r="B220" t="s">
+        <v>44</v>
+      </c>
       <c r="E220" t="s">
         <v>1433</v>
       </c>
@@ -9728,6 +9789,9 @@
       <c r="A222" s="1" t="s">
         <v>1287</v>
       </c>
+      <c r="B222" t="s">
+        <v>78</v>
+      </c>
       <c r="E222" t="s">
         <v>1434</v>
       </c>
@@ -9745,6 +9809,9 @@
       <c r="A223" s="1" t="s">
         <v>1304</v>
       </c>
+      <c r="B223" t="s">
+        <v>44</v>
+      </c>
       <c r="E223" t="s">
         <v>1435</v>
       </c>
@@ -9762,6 +9829,9 @@
       <c r="A224" s="1" t="s">
         <v>1293</v>
       </c>
+      <c r="B224" t="s">
+        <v>78</v>
+      </c>
       <c r="E224" t="s">
         <v>1436</v>
       </c>
@@ -9779,6 +9849,9 @@
       <c r="A225" s="1" t="s">
         <v>1310</v>
       </c>
+      <c r="B225" t="s">
+        <v>44</v>
+      </c>
       <c r="E225" t="s">
         <v>1437</v>
       </c>
@@ -9796,6 +9869,9 @@
       <c r="A226" s="1" t="s">
         <v>1283</v>
       </c>
+      <c r="B226" t="s">
+        <v>78</v>
+      </c>
       <c r="E226" t="s">
         <v>1438</v>
       </c>
@@ -9813,6 +9889,9 @@
       <c r="A227" s="1" t="s">
         <v>1300</v>
       </c>
+      <c r="B227" t="s">
+        <v>44</v>
+      </c>
       <c r="E227" t="s">
         <v>1439</v>
       </c>
@@ -9876,6 +9955,9 @@
       <c r="A230" s="1" t="s">
         <v>1286</v>
       </c>
+      <c r="B230" t="s">
+        <v>78</v>
+      </c>
       <c r="E230" t="s">
         <v>1440</v>
       </c>
@@ -9893,6 +9975,9 @@
       <c r="A231" s="1" t="s">
         <v>1302</v>
       </c>
+      <c r="B231" t="s">
+        <v>44</v>
+      </c>
       <c r="E231" t="s">
         <v>1210</v>
       </c>
@@ -9910,6 +9995,9 @@
       <c r="A232" s="1" t="s">
         <v>1285</v>
       </c>
+      <c r="B232" t="s">
+        <v>78</v>
+      </c>
       <c r="E232" t="s">
         <v>1441</v>
       </c>
@@ -9927,6 +10015,9 @@
       <c r="A233" s="1" t="s">
         <v>1303</v>
       </c>
+      <c r="B233" t="s">
+        <v>44</v>
+      </c>
       <c r="E233" t="s">
         <v>1442</v>
       </c>
@@ -9944,6 +10035,9 @@
       <c r="A234" s="1" t="s">
         <v>1280</v>
       </c>
+      <c r="B234" t="s">
+        <v>78</v>
+      </c>
       <c r="E234" t="s">
         <v>1443</v>
       </c>
@@ -9961,6 +10055,9 @@
       <c r="A235" s="1" t="s">
         <v>1297</v>
       </c>
+      <c r="B235" t="s">
+        <v>44</v>
+      </c>
       <c r="E235" t="s">
         <v>1444</v>
       </c>
@@ -10001,6 +10098,9 @@
       <c r="A237" s="1" t="s">
         <v>1289</v>
       </c>
+      <c r="B237" t="s">
+        <v>78</v>
+      </c>
       <c r="E237" t="s">
         <v>1445</v>
       </c>
@@ -10018,6 +10118,9 @@
       <c r="A238" s="1" t="s">
         <v>1306</v>
       </c>
+      <c r="B238" t="s">
+        <v>44</v>
+      </c>
       <c r="E238" t="s">
         <v>1446</v>
       </c>
@@ -10035,6 +10138,9 @@
       <c r="A239" s="1" t="s">
         <v>1290</v>
       </c>
+      <c r="B239" t="s">
+        <v>78</v>
+      </c>
       <c r="E239" t="s">
         <v>1447</v>
       </c>
@@ -10052,6 +10158,9 @@
       <c r="A240" s="1" t="s">
         <v>1307</v>
       </c>
+      <c r="B240" t="s">
+        <v>44</v>
+      </c>
       <c r="E240" t="s">
         <v>1448</v>
       </c>
@@ -10069,6 +10178,9 @@
       <c r="A241" s="1" t="s">
         <v>1288</v>
       </c>
+      <c r="B241" t="s">
+        <v>78</v>
+      </c>
       <c r="E241" t="s">
         <v>1449</v>
       </c>
@@ -10086,6 +10198,9 @@
       <c r="A242" s="1" t="s">
         <v>1305</v>
       </c>
+      <c r="B242" t="s">
+        <v>44</v>
+      </c>
       <c r="E242" t="s">
         <v>1450</v>
       </c>
@@ -10715,6 +10830,9 @@
     <row r="272" spans="1:11">
       <c r="A272" s="1" t="s">
         <v>1311</v>
+      </c>
+      <c r="B272" t="s">
+        <v>44</v>
       </c>
       <c r="E272" t="s">
         <v>1417</v>
@@ -11087,4 +11205,2181 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K92"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="6" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="7.5" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="46.1640625" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>832</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>635</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1211</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="I2" t="s">
+        <v>458</v>
+      </c>
+      <c r="J2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1137</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>614</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1201</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="I4" t="s">
+        <v>437</v>
+      </c>
+      <c r="J4" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>568</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1221</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="I5" t="s">
+        <v>750</v>
+      </c>
+      <c r="J5" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>604</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1194</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="I6" t="s">
+        <v>427</v>
+      </c>
+      <c r="J6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>603</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1217</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="I7" t="s">
+        <v>785</v>
+      </c>
+      <c r="J7" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1145</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" t="s">
+        <v>152</v>
+      </c>
+      <c r="J8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>581</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="I9" t="s">
+        <v>763</v>
+      </c>
+      <c r="J9" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>624</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1207</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="I10" t="s">
+        <v>447</v>
+      </c>
+      <c r="J10" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>580</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="I11" t="s">
+        <v>762</v>
+      </c>
+      <c r="J11" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>623</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1206</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="I12" t="s">
+        <v>446</v>
+      </c>
+      <c r="J12" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>571</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1222</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="I13" t="s">
+        <v>753</v>
+      </c>
+      <c r="J13" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>582</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1220</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="I14" t="s">
+        <v>764</v>
+      </c>
+      <c r="J14" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>625</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1208</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="I15" t="s">
+        <v>448</v>
+      </c>
+      <c r="J15" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>648</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1149</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I16" t="s">
+        <v>251</v>
+      </c>
+      <c r="J16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>609</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1198</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="I17" t="s">
+        <v>432</v>
+      </c>
+      <c r="J17" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>607</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1196</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="I18" t="s">
+        <v>430</v>
+      </c>
+      <c r="J18" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H19" s="1">
+        <v>30</v>
+      </c>
+      <c r="I19" t="s">
+        <v>118</v>
+      </c>
+      <c r="J19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H20" s="1">
+        <v>31</v>
+      </c>
+      <c r="I20" t="s">
+        <v>109</v>
+      </c>
+      <c r="J20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1128</v>
+      </c>
+      <c r="H21" s="1">
+        <v>32</v>
+      </c>
+      <c r="I21" t="s">
+        <v>110</v>
+      </c>
+      <c r="J21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1129</v>
+      </c>
+      <c r="H22" s="1">
+        <v>33</v>
+      </c>
+      <c r="I22" t="s">
+        <v>111</v>
+      </c>
+      <c r="J22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1130</v>
+      </c>
+      <c r="H23" s="1">
+        <v>34</v>
+      </c>
+      <c r="I23" t="s">
+        <v>112</v>
+      </c>
+      <c r="J23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="1">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H24" s="1">
+        <v>35</v>
+      </c>
+      <c r="I24" t="s">
+        <v>113</v>
+      </c>
+      <c r="J24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="1">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="1">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H25" s="1">
+        <v>36</v>
+      </c>
+      <c r="I25" t="s">
+        <v>114</v>
+      </c>
+      <c r="J25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="1">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="1">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1133</v>
+      </c>
+      <c r="H26" s="1">
+        <v>37</v>
+      </c>
+      <c r="I26" t="s">
+        <v>115</v>
+      </c>
+      <c r="J26" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="1">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1134</v>
+      </c>
+      <c r="H27" s="1">
+        <v>38</v>
+      </c>
+      <c r="I27" t="s">
+        <v>116</v>
+      </c>
+      <c r="J27" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="1">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="1">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1135</v>
+      </c>
+      <c r="H28" s="1">
+        <v>39</v>
+      </c>
+      <c r="I28" t="s">
+        <v>117</v>
+      </c>
+      <c r="J28" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" t="s">
+        <v>565</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1215</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="I29" t="s">
+        <v>747</v>
+      </c>
+      <c r="J29" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>657</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1158</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I30" t="s">
+        <v>260</v>
+      </c>
+      <c r="J30" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>573</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1216</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="I31" t="s">
+        <v>755</v>
+      </c>
+      <c r="J31" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
+        <v>611</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1199</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="I32" t="s">
+        <v>434</v>
+      </c>
+      <c r="J32" t="s">
+        <v>476</v>
+      </c>
+      <c r="K32" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" t="s">
+        <v>658</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1159</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I33" t="s">
+        <v>261</v>
+      </c>
+      <c r="J33" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>606</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1195</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I34" t="s">
+        <v>429</v>
+      </c>
+      <c r="J34" t="s">
+        <v>471</v>
+      </c>
+      <c r="K34" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>620</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1203</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="I35" t="s">
+        <v>443</v>
+      </c>
+      <c r="J35" t="s">
+        <v>485</v>
+      </c>
+      <c r="K35" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" t="s">
+        <v>559</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1213</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="I36" t="s">
+        <v>741</v>
+      </c>
+      <c r="J36" t="s">
+        <v>787</v>
+      </c>
+      <c r="K36" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="1">
+        <v>61</v>
+      </c>
+      <c r="I37" t="s">
+        <v>134</v>
+      </c>
+      <c r="J37" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" t="s">
+        <v>857</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1260</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="I38" t="s">
+        <v>868</v>
+      </c>
+      <c r="J38" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" t="s">
+        <v>915</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1224</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="I39" t="s">
+        <v>903</v>
+      </c>
+      <c r="J39" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1272</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I40" t="s">
+        <v>1013</v>
+      </c>
+      <c r="J40" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1268</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="I41" t="s">
+        <v>951</v>
+      </c>
+      <c r="J41" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" t="s">
+        <v>636</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1212</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="I42" t="s">
+        <v>459</v>
+      </c>
+      <c r="J42" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1274</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="I43" t="s">
+        <v>1031</v>
+      </c>
+      <c r="J43" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" t="s">
+        <v>626</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1209</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="I44" t="s">
+        <v>449</v>
+      </c>
+      <c r="J44" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" s="1">
+        <v>62</v>
+      </c>
+      <c r="I45" t="s">
+        <v>148</v>
+      </c>
+      <c r="J45" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" t="s">
+        <v>35</v>
+      </c>
+      <c r="H46" s="1">
+        <v>63</v>
+      </c>
+      <c r="I46" t="s">
+        <v>146</v>
+      </c>
+      <c r="J46" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B47" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" t="s">
+        <v>639</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1276</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="I47" t="s">
+        <v>462</v>
+      </c>
+      <c r="J47" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48" s="1">
+        <v>64</v>
+      </c>
+      <c r="I48" t="s">
+        <v>136</v>
+      </c>
+      <c r="J48" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" s="1">
+        <v>65</v>
+      </c>
+      <c r="I49" t="s">
+        <v>123</v>
+      </c>
+      <c r="J49" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B50" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" t="s">
+        <v>853</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1253</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="I50" t="s">
+        <v>864</v>
+      </c>
+      <c r="J50" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="B51" t="s">
+        <v>44</v>
+      </c>
+      <c r="D51" t="s">
+        <v>911</v>
+      </c>
+      <c r="E51" t="s">
+        <v>1255</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="I51" t="s">
+        <v>899</v>
+      </c>
+      <c r="J51" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="B52" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1256</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="I52" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J52" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="B53" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1254</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="I53" t="s">
+        <v>946</v>
+      </c>
+      <c r="J53" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54" t="s">
+        <v>25</v>
+      </c>
+      <c r="H54" s="1">
+        <v>66</v>
+      </c>
+      <c r="I54" t="s">
+        <v>137</v>
+      </c>
+      <c r="J54" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" t="s">
+        <v>44</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" t="s">
+        <v>26</v>
+      </c>
+      <c r="H55" s="1">
+        <v>67</v>
+      </c>
+      <c r="I55" t="s">
+        <v>138</v>
+      </c>
+      <c r="J55" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" t="s">
+        <v>27</v>
+      </c>
+      <c r="H56" s="1">
+        <v>68</v>
+      </c>
+      <c r="I56" t="s">
+        <v>139</v>
+      </c>
+      <c r="J56" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" t="s">
+        <v>16</v>
+      </c>
+      <c r="H57" s="1">
+        <v>69</v>
+      </c>
+      <c r="I57" t="s">
+        <v>128</v>
+      </c>
+      <c r="J57" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="B58" t="s">
+        <v>44</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E58" t="s">
+        <v>1270</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I58" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J58" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="B59" t="s">
+        <v>44</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E59" t="s">
+        <v>1266</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="I59" t="s">
+        <v>949</v>
+      </c>
+      <c r="J59" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="B60" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" t="s">
+        <v>913</v>
+      </c>
+      <c r="E60" t="s">
+        <v>1262</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="I60" t="s">
+        <v>901</v>
+      </c>
+      <c r="J60" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="B61" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61" t="s">
+        <v>855</v>
+      </c>
+      <c r="E61" t="s">
+        <v>1258</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="I61" t="s">
+        <v>866</v>
+      </c>
+      <c r="J61" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" t="s">
+        <v>44</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" t="s">
+        <v>28</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I62" t="s">
+        <v>140</v>
+      </c>
+      <c r="J62" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B63" t="s">
+        <v>44</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E63" t="s">
+        <v>29</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I63" t="s">
+        <v>135</v>
+      </c>
+      <c r="J63" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" t="s">
+        <v>44</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E64" t="s">
+        <v>30</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I64" t="s">
+        <v>141</v>
+      </c>
+      <c r="J64" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" t="s">
+        <v>44</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E65" t="s">
+        <v>39</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I65" t="s">
+        <v>150</v>
+      </c>
+      <c r="J65" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66" t="s">
+        <v>44</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" t="s">
+        <v>38</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I66" t="s">
+        <v>149</v>
+      </c>
+      <c r="J66" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="B67" t="s">
+        <v>44</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E67" t="s">
+        <v>1275</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="I67" t="s">
+        <v>1032</v>
+      </c>
+      <c r="J67" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68" t="s">
+        <v>44</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" t="s">
+        <v>17</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I68" t="s">
+        <v>129</v>
+      </c>
+      <c r="J68" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="B69" t="s">
+        <v>44</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E69" t="s">
+        <v>1271</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="I69" t="s">
+        <v>1012</v>
+      </c>
+      <c r="J69" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="B70" t="s">
+        <v>44</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1267</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="I70" t="s">
+        <v>950</v>
+      </c>
+      <c r="J70" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B71" t="s">
+        <v>44</v>
+      </c>
+      <c r="D71" t="s">
+        <v>856</v>
+      </c>
+      <c r="E71" t="s">
+        <v>1259</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="I71" t="s">
+        <v>867</v>
+      </c>
+      <c r="J71" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="B72" t="s">
+        <v>44</v>
+      </c>
+      <c r="D72" t="s">
+        <v>914</v>
+      </c>
+      <c r="E72" t="s">
+        <v>1263</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="I72" t="s">
+        <v>902</v>
+      </c>
+      <c r="J72" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B73" t="s">
+        <v>44</v>
+      </c>
+      <c r="D73" t="s">
+        <v>616</v>
+      </c>
+      <c r="E73" t="s">
+        <v>1202</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="I73" t="s">
+        <v>439</v>
+      </c>
+      <c r="J73" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B74" t="s">
+        <v>44</v>
+      </c>
+      <c r="D74" t="s">
+        <v>621</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1205</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="I74" t="s">
+        <v>444</v>
+      </c>
+      <c r="J74" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="B75" t="s">
+        <v>44</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E75" t="s">
+        <v>1273</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="I75" t="s">
+        <v>1030</v>
+      </c>
+      <c r="J75" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76" t="s">
+        <v>44</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E76" t="s">
+        <v>18</v>
+      </c>
+      <c r="H76" s="1">
+        <v>70</v>
+      </c>
+      <c r="I76" t="s">
+        <v>130</v>
+      </c>
+      <c r="J76" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B77" t="s">
+        <v>44</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>9</v>
+      </c>
+      <c r="H77" s="1">
+        <v>71</v>
+      </c>
+      <c r="I77" t="s">
+        <v>121</v>
+      </c>
+      <c r="J77" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" t="s">
+        <v>44</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" t="s">
+        <v>12</v>
+      </c>
+      <c r="H78" s="1">
+        <v>72</v>
+      </c>
+      <c r="I78" t="s">
+        <v>124</v>
+      </c>
+      <c r="J78" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79" t="s">
+        <v>44</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E79" t="s">
+        <v>23</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I79" t="s">
+        <v>135</v>
+      </c>
+      <c r="J79" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B80" t="s">
+        <v>44</v>
+      </c>
+      <c r="D80" t="s">
+        <v>627</v>
+      </c>
+      <c r="E80" t="s">
+        <v>1210</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="I80" t="s">
+        <v>450</v>
+      </c>
+      <c r="J80" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" t="s">
+        <v>44</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" t="s">
+        <v>13</v>
+      </c>
+      <c r="H81" s="1">
+        <v>74</v>
+      </c>
+      <c r="I81" t="s">
+        <v>125</v>
+      </c>
+      <c r="J81" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B82" t="s">
+        <v>44</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E82" t="s">
+        <v>15</v>
+      </c>
+      <c r="H82" s="1">
+        <v>75</v>
+      </c>
+      <c r="I82" t="s">
+        <v>127</v>
+      </c>
+      <c r="J82" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="B83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E83" t="s">
+        <v>1269</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="I83" t="s">
+        <v>1010</v>
+      </c>
+      <c r="J83" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="B84" t="s">
+        <v>44</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E84" t="s">
+        <v>1265</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="I84" t="s">
+        <v>948</v>
+      </c>
+      <c r="J84" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="B85" t="s">
+        <v>44</v>
+      </c>
+      <c r="D85" t="s">
+        <v>854</v>
+      </c>
+      <c r="E85" t="s">
+        <v>1257</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="I85" t="s">
+        <v>865</v>
+      </c>
+      <c r="J85" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="B86" t="s">
+        <v>44</v>
+      </c>
+      <c r="D86" t="s">
+        <v>912</v>
+      </c>
+      <c r="E86" t="s">
+        <v>1261</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="I86" t="s">
+        <v>900</v>
+      </c>
+      <c r="J86" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B87" t="s">
+        <v>44</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E87" t="s">
+        <v>36</v>
+      </c>
+      <c r="H87" s="1">
+        <v>76</v>
+      </c>
+      <c r="I87" t="s">
+        <v>147</v>
+      </c>
+      <c r="J87" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" t="s">
+        <v>44</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" t="s">
+        <v>10</v>
+      </c>
+      <c r="H88" s="1">
+        <v>77</v>
+      </c>
+      <c r="I88" t="s">
+        <v>122</v>
+      </c>
+      <c r="J88" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B89" t="s">
+        <v>44</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E89" t="s">
+        <v>34</v>
+      </c>
+      <c r="H89" s="1">
+        <v>78</v>
+      </c>
+      <c r="I89" t="s">
+        <v>145</v>
+      </c>
+      <c r="J89" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B90" t="s">
+        <v>44</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E90" t="s">
+        <v>14</v>
+      </c>
+      <c r="H90" s="1">
+        <v>79</v>
+      </c>
+      <c r="I90" t="s">
+        <v>126</v>
+      </c>
+      <c r="J90" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="B91" t="s">
+        <v>44</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1112</v>
+      </c>
+      <c r="E91" t="s">
+        <v>1264</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="I91" t="s">
+        <v>947</v>
+      </c>
+      <c r="J91" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" t="s">
+        <v>44</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E92" t="s">
+        <v>33</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I92" t="s">
+        <v>144</v>
+      </c>
+      <c r="J92" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:K144">
+    <sortCondition ref="E2:E144"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>